<commit_message>
Update fix bug ar sum
</commit_message>
<xml_diff>
--- a/WebAPI/eFMS.API.SystemWeb/eFMS.API.ReportData/eFMS.API.ReportData/FormatExcel/TemplateExport/AccountReceivable/AR_SUMMARY_TEMPLATE.xlsx
+++ b/WebAPI/eFMS.API.SystemWeb/eFMS.API.ReportData/eFMS.API.ReportData/FormatExcel/TemplateExport/AccountReceivable/AR_SUMMARY_TEMPLATE.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Code_Khoa\efms-dev\eFMS-WebApp\WebAPI\eFMS.API.SystemWeb\eFMS.API.ReportData\eFMS.API.ReportData\FormatExcel\TemplateExport\AccountReceivable\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Code_Khoa\efms-prod\eFMS-WebApp\WebAPI\eFMS.API.SystemWeb\eFMS.API.ReportData\eFMS.API.ReportData\FormatExcel\TemplateExport\AccountReceivable\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2250" windowWidth="28770" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="4950" windowWidth="28770" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="AR SUMMARY" sheetId="1" r:id="rId1"/>
@@ -362,9 +362,6 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
@@ -373,6 +370,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -664,7 +664,7 @@
       <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="N21" sqref="N21"/>
+      <selection pane="bottomRight" activeCell="R25" sqref="R25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -851,34 +851,34 @@
       <c r="C3" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="F3" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="G3" s="15" t="s">
+      <c r="G3" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="H3" s="15" t="s">
+      <c r="H3" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="15" t="s">
+      <c r="I3" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="J3" s="15" t="s">
+      <c r="J3" s="14" t="s">
         <v>41</v>
       </c>
       <c r="K3" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="L3" s="15" t="s">
+      <c r="L3" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="M3" s="15" t="s">
+      <c r="M3" s="14" t="s">
         <v>30</v>
       </c>
       <c r="N3" s="8" t="s">
@@ -906,34 +906,34 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:21" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="17"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="18"/>
+    <row r="6" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="16"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="17"/>
     </row>
-    <row r="7" spans="1:21" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="20"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="18"/>
+    <row r="7" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="19"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="17"/>
     </row>
-    <row r="8" spans="1:21" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="20"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="18"/>
+    <row r="8" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="19"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="17"/>
     </row>
-    <row r="9" spans="1:21" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="20"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="18"/>
+    <row r="9" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="19"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="17"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:U3"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
++ thêm shipmentType vào formContract,  email contract,  report AR summary,
</commit_message>
<xml_diff>
--- a/WebAPI/eFMS.API.SystemWeb/eFMS.API.ReportData/eFMS.API.ReportData/FormatExcel/TemplateExport/AccountReceivable/AR_SUMMARY_TEMPLATE.xlsx
+++ b/WebAPI/eFMS.API.SystemWeb/eFMS.API.ReportData/eFMS.API.ReportData/FormatExcel/TemplateExport/AccountReceivable/AR_SUMMARY_TEMPLATE.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Code_Khoa\efms-uat\eFMS-WebApp\WebAPI\eFMS.API.SystemWeb\eFMS.API.ReportData\eFMS.API.ReportData\FormatExcel\TemplateExport\AccountReceivable\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\eFMS-WebApp\WebAPI\eFMS.API.SystemWeb\eFMS.API.ReportData\eFMS.API.ReportData\FormatExcel\TemplateExport\AccountReceivable\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,9 +15,9 @@
     <sheet name="AR SUMMARY" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'AR SUMMARY'!$A$2:$U$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'AR SUMMARY'!$A$2:$V$3</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" iterate="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>Parent Partner</t>
   </si>
@@ -179,6 +179,12 @@
   </si>
   <si>
     <t>{Over30Days}</t>
+  </si>
+  <si>
+    <t>Shipment Type</t>
+  </si>
+  <si>
+    <t>{ShipmentType}</t>
   </si>
 </sst>
 </file>
@@ -657,13 +663,13 @@
   <sheetPr>
     <tabColor rgb="FFC00000"/>
   </sheetPr>
-  <dimension ref="A1:U9"/>
+  <dimension ref="A1:V9"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="4" ySplit="2" topLeftCell="Q3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="Y20" sqref="Y20"/>
+      <selection pane="bottomRight" activeCell="S4" sqref="S4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -686,31 +692,32 @@
     <col min="16" max="16" width="14" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="39" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="28.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="30" style="1" customWidth="1"/>
-    <col min="23" max="23" width="16" style="1" customWidth="1"/>
-    <col min="24" max="24" width="14" style="1" customWidth="1"/>
-    <col min="25" max="25" width="18" style="1" customWidth="1"/>
-    <col min="26" max="26" width="10" style="1" customWidth="1"/>
-    <col min="27" max="27" width="12" style="1" customWidth="1"/>
-    <col min="28" max="28" width="8" style="1" customWidth="1"/>
-    <col min="29" max="29" width="10" style="1" customWidth="1"/>
-    <col min="30" max="30" width="14" style="1" customWidth="1"/>
-    <col min="31" max="31" width="10" style="1" customWidth="1"/>
-    <col min="32" max="32" width="15" style="1" customWidth="1"/>
-    <col min="33" max="33" width="12" style="1" customWidth="1"/>
-    <col min="34" max="35" width="10" style="1" customWidth="1"/>
-    <col min="36" max="36" width="30" style="1" customWidth="1"/>
-    <col min="37" max="37" width="15" style="1" customWidth="1"/>
-    <col min="38" max="38" width="18" style="1" customWidth="1"/>
-    <col min="39" max="39" width="20" style="1" customWidth="1"/>
-    <col min="40" max="40" width="25" style="1" customWidth="1"/>
-    <col min="41" max="16384" width="8.85546875" style="1"/>
+    <col min="19" max="19" width="39" style="1" customWidth="1"/>
+    <col min="20" max="20" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="28.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="30" style="1" customWidth="1"/>
+    <col min="24" max="24" width="16" style="1" customWidth="1"/>
+    <col min="25" max="25" width="14" style="1" customWidth="1"/>
+    <col min="26" max="26" width="18" style="1" customWidth="1"/>
+    <col min="27" max="27" width="10" style="1" customWidth="1"/>
+    <col min="28" max="28" width="12" style="1" customWidth="1"/>
+    <col min="29" max="29" width="8" style="1" customWidth="1"/>
+    <col min="30" max="30" width="10" style="1" customWidth="1"/>
+    <col min="31" max="31" width="14" style="1" customWidth="1"/>
+    <col min="32" max="32" width="10" style="1" customWidth="1"/>
+    <col min="33" max="33" width="15" style="1" customWidth="1"/>
+    <col min="34" max="34" width="12" style="1" customWidth="1"/>
+    <col min="35" max="36" width="10" style="1" customWidth="1"/>
+    <col min="37" max="37" width="30" style="1" customWidth="1"/>
+    <col min="38" max="38" width="15" style="1" customWidth="1"/>
+    <col min="39" max="39" width="18" style="1" customWidth="1"/>
+    <col min="40" max="40" width="20" style="1" customWidth="1"/>
+    <col min="41" max="41" width="25" style="1" customWidth="1"/>
+    <col min="42" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>19</v>
       </c>
@@ -766,16 +773,19 @@
         <v>3</v>
       </c>
       <c r="S1" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="T1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="T1" s="11" t="s">
+      <c r="U1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="U1" s="10" t="s">
+      <c r="V1" s="10" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:21" s="8" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:22" s="8" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="A2" s="9">
         <v>1</v>
       </c>
@@ -830,17 +840,18 @@
       <c r="R2" s="9">
         <v>18</v>
       </c>
-      <c r="S2" s="9">
+      <c r="S2" s="9"/>
+      <c r="T2" s="9">
         <v>19</v>
       </c>
-      <c r="T2" s="9">
+      <c r="U2" s="9">
         <v>20</v>
       </c>
-      <c r="U2" s="9">
+      <c r="V2" s="9">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>39</v>
       </c>
@@ -895,42 +906,45 @@
       <c r="R3" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="S3" s="5" t="s">
+      <c r="S3" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="T3" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="T3" s="4" t="s">
+      <c r="U3" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="U3" s="3" t="s">
+      <c r="V3" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="14"/>
       <c r="C6" s="15"/>
       <c r="D6" s="16"/>
       <c r="E6" s="15"/>
     </row>
-    <row r="7" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="17"/>
       <c r="C7" s="15"/>
       <c r="D7" s="16"/>
       <c r="E7" s="15"/>
     </row>
-    <row r="8" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B8" s="17"/>
       <c r="C8" s="15"/>
       <c r="D8" s="16"/>
       <c r="E8" s="15"/>
     </row>
-    <row r="9" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B9" s="17"/>
       <c r="C9" s="15"/>
       <c r="D9" s="16"/>
       <c r="E9" s="15"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:U3"/>
+  <autoFilter ref="A2:V3"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>

</xml_diff>